<commit_message>
Basic map 7 Sep-1
</commit_message>
<xml_diff>
--- a/Updated_From_DEV.xlsx
+++ b/Updated_From_DEV.xlsx
@@ -7850,7 +7850,7 @@
         <v>50.6745006469311</v>
       </c>
       <c r="K9" s="10">
-        <v>50.6745006469311</v>
+        <v>-100.815510962484</v>
       </c>
       <c r="L9" t="s" s="9">
         <v>84</v>
@@ -7922,10 +7922,10 @@
         <v>89</v>
       </c>
       <c r="J10" s="10">
-        <v>49.2444237419695</v>
+        <v>53.9121049030002</v>
       </c>
       <c r="K10" s="10">
-        <v>-123.124303003041</v>
+        <v>-122.763977018131</v>
       </c>
       <c r="L10" t="s" s="9">
         <v>90</v>

</xml_diff>

<commit_message>
Basic map 7 Sep-3
</commit_message>
<xml_diff>
--- a/Updated_From_DEV.xlsx
+++ b/Updated_From_DEV.xlsx
@@ -17478,16 +17478,16 @@
       <c r="H136" s="10">
         <v>0</v>
       </c>
-      <c r="I136" t="s" s="9">
+      <c r="I136" s="11"/>
+      <c r="J136" s="10">
+        <v>0</v>
+      </c>
+      <c r="K136" s="10">
+        <v>0</v>
+      </c>
+      <c r="L136" t="s" s="9">
         <v>946</v>
       </c>
-      <c r="J136" s="10">
-        <v>0</v>
-      </c>
-      <c r="K136" s="10">
-        <v>0</v>
-      </c>
-      <c r="L136" s="11"/>
       <c r="M136" s="10">
         <v>1984</v>
       </c>
@@ -29382,7 +29382,7 @@
     <hyperlink ref="L134" r:id="rId202" location="" tooltip="" display="https://www.cbc.ca/missingandmurdered/mmiw/profiles/jamie-nora-mcguire"/>
     <hyperlink ref="I135" r:id="rId203" location="" tooltip="" display="https://www.cbc.ca/missingandmurdered/mmiw/profiles/jane-bernard"/>
     <hyperlink ref="L135" r:id="rId204" location="" tooltip="" display="https://www.cbc.ca/missingandmurdered/mmiw/profiles/jane-bernard"/>
-    <hyperlink ref="I136" r:id="rId205" location="" tooltip="" display="https://www.cbc.ca/missingandmurdered/mmiw/profiles/jane-louise-sutherland"/>
+    <hyperlink ref="L136" r:id="rId205" location="" tooltip="" display="https://www.cbc.ca/missingandmurdered/mmiw/profiles/jane-louise-sutherland"/>
     <hyperlink ref="I137" r:id="rId206" location="" tooltip="" display="https://www.cbc.ca/missingandmurdered/mmiw/profiles/janet-gail-henry"/>
     <hyperlink ref="I138" r:id="rId207" location="" tooltip="" display="https://www.cbc.ca/missingandmurdered/mmiw/profiles/janet-sylvestre"/>
     <hyperlink ref="L138" r:id="rId208" location="" tooltip="" display="https://www.cbc.ca/missingandmurdered/mmiw/profiles/janet-sylvestre"/>

</xml_diff>